<commit_message>
update after fixing error of using two terms to describe adolescent
</commit_message>
<xml_diff>
--- a/data/data-without-outliers.xlsx
+++ b/data/data-without-outliers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcc/Insync/geiser@alumni.usp.br/Google Drive/Workspace/nature/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcc/Insync/geiser@alumni.usp.br/Google Drive/Workspace/meta-analysis-gender-st/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6042F7F0-F832-AD4A-8C1E-7C5ED4180585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FFC919-580F-CD48-BB1A-BBB5ACE5C829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13940" activeTab="3" xr2:uid="{5F27C989-7FC7-5A40-902F-A9E477438C24}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13940" activeTab="4" xr2:uid="{5F27C989-7FC7-5A40-902F-A9E477438C24}"/>
   </bookViews>
   <sheets>
     <sheet name="perform-cond-descriptive" sheetId="13" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="82">
   <si>
     <t>Author</t>
   </si>
@@ -189,9 +189,6 @@
   </si>
   <si>
     <t>factor</t>
-  </si>
-  <si>
-    <t>adolescence</t>
   </si>
   <si>
     <t>adult</t>
@@ -707,7 +704,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
         <v>37</v>
@@ -719,10 +716,10 @@
         <v>39</v>
       </c>
       <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
         <v>59</v>
-      </c>
-      <c r="H1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1495,7 +1492,7 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D32">
         <v>38</v>
@@ -1521,7 +1518,7 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D33">
         <v>29</v>
@@ -1573,7 +1570,7 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E1" t="s">
         <v>37</v>
@@ -1585,10 +1582,10 @@
         <v>39</v>
       </c>
       <c r="H1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" t="s">
         <v>59</v>
-      </c>
-      <c r="I1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1599,7 +1596,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
         <v>46</v>
@@ -1628,7 +1625,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
         <v>46</v>
@@ -1657,7 +1654,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
         <v>46</v>
@@ -1686,7 +1683,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
         <v>46</v>
@@ -1715,7 +1712,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
@@ -1744,7 +1741,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
         <v>46</v>
@@ -1773,7 +1770,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
         <v>46</v>
@@ -1802,7 +1799,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -1831,7 +1828,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
         <v>46</v>
@@ -1860,7 +1857,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
         <v>46</v>
@@ -1889,7 +1886,7 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
         <v>46</v>
@@ -1918,7 +1915,7 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
         <v>46</v>
@@ -1947,7 +1944,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
@@ -1976,7 +1973,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
         <v>46</v>
@@ -2005,7 +2002,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
         <v>46</v>
@@ -2034,7 +2031,7 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
         <v>46</v>
@@ -2063,7 +2060,7 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
         <v>46</v>
@@ -2092,7 +2089,7 @@
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
         <v>46</v>
@@ -2121,7 +2118,7 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D20" t="s">
         <v>46</v>
@@ -2150,7 +2147,7 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
         <v>46</v>
@@ -2179,7 +2176,7 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22" t="s">
         <v>46</v>
@@ -2208,7 +2205,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D23" t="s">
         <v>46</v>
@@ -2237,7 +2234,7 @@
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D24" t="s">
         <v>46</v>
@@ -2266,7 +2263,7 @@
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25" t="s">
         <v>46</v>
@@ -2295,7 +2292,7 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
         <v>46</v>
@@ -2324,7 +2321,7 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27" t="s">
         <v>46</v>
@@ -2353,7 +2350,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
         <v>46</v>
@@ -2382,7 +2379,7 @@
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D29" t="s">
         <v>46</v>
@@ -2411,7 +2408,7 @@
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30" t="s">
         <v>46</v>
@@ -2440,7 +2437,7 @@
         <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D31" t="s">
         <v>46</v>
@@ -2469,7 +2466,7 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D32" t="s">
         <v>46</v>
@@ -2498,7 +2495,7 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D33" t="s">
         <v>46</v>
@@ -2527,7 +2524,7 @@
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34" t="s">
         <v>46</v>
@@ -2556,7 +2553,7 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D35" t="s">
         <v>46</v>
@@ -2585,7 +2582,7 @@
         <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D36" t="s">
         <v>46</v>
@@ -2614,7 +2611,7 @@
         <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D37" t="s">
         <v>46</v>
@@ -2643,7 +2640,7 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D38" t="s">
         <v>46</v>
@@ -2672,7 +2669,7 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D39" t="s">
         <v>46</v>
@@ -2701,7 +2698,7 @@
         <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D40" t="s">
         <v>46</v>
@@ -2730,7 +2727,7 @@
         <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D41" t="s">
         <v>46</v>
@@ -2759,7 +2756,7 @@
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D42" t="s">
         <v>46</v>
@@ -2788,7 +2785,7 @@
         <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D43" t="s">
         <v>46</v>
@@ -2817,7 +2814,7 @@
         <v>3</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>46</v>
@@ -2840,7 +2837,7 @@
         <v>6</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>46</v>
@@ -2863,7 +2860,7 @@
         <v>7</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>46</v>
@@ -2886,7 +2883,7 @@
         <v>3</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>46</v>
@@ -2909,7 +2906,7 @@
         <v>6</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>46</v>
@@ -2932,7 +2929,7 @@
         <v>7</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>46</v>
@@ -2955,7 +2952,7 @@
         <v>6</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>46</v>
@@ -2984,7 +2981,7 @@
         <v>6</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>46</v>
@@ -3013,7 +3010,7 @@
         <v>7</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>46</v>
@@ -3042,7 +3039,7 @@
         <v>7</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>46</v>
@@ -3071,7 +3068,7 @@
         <v>3</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>46</v>
@@ -3100,7 +3097,7 @@
         <v>3</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>46</v>
@@ -3129,7 +3126,7 @@
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D56" t="s">
         <v>46</v>
@@ -3158,7 +3155,7 @@
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D57" t="s">
         <v>46</v>
@@ -3187,7 +3184,7 @@
         <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D58" t="s">
         <v>46</v>
@@ -3216,7 +3213,7 @@
         <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D59" t="s">
         <v>46</v>
@@ -3245,7 +3242,7 @@
         <v>7</v>
       </c>
       <c r="C60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D60" t="s">
         <v>46</v>
@@ -3274,7 +3271,7 @@
         <v>7</v>
       </c>
       <c r="C61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D61" t="s">
         <v>46</v>
@@ -3306,7 +3303,7 @@
         <v>42</v>
       </c>
       <c r="D62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E62">
         <v>30</v>
@@ -3335,7 +3332,7 @@
         <v>41</v>
       </c>
       <c r="D63" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E63">
         <v>7</v>
@@ -3364,7 +3361,7 @@
         <v>42</v>
       </c>
       <c r="D64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E64">
         <v>22</v>
@@ -3393,7 +3390,7 @@
         <v>41</v>
       </c>
       <c r="D65" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E65">
         <v>8</v>
@@ -3449,10 +3446,10 @@
         <v>38</v>
       </c>
       <c r="F1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" t="s">
         <v>78</v>
-      </c>
-      <c r="G1" t="s">
-        <v>79</v>
       </c>
       <c r="H1" t="s">
         <v>39</v>
@@ -4305,7 +4302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1583BFA1-A12B-054D-B239-FE6D88A44BA2}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -4331,10 +4328,10 @@
         <v>38</v>
       </c>
       <c r="G1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" t="s">
         <v>78</v>
-      </c>
-      <c r="H1" t="s">
-        <v>79</v>
       </c>
       <c r="I1" t="s">
         <v>39</v>
@@ -4354,7 +4351,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2">
         <v>13</v>
@@ -4389,7 +4386,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3">
         <v>21</v>
@@ -4424,7 +4421,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4">
         <v>7</v>
@@ -4459,7 +4456,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5">
         <v>18</v>
@@ -4494,7 +4491,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -4529,7 +4526,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7">
         <v>19</v>
@@ -4564,7 +4561,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8">
         <v>11</v>
@@ -4599,7 +4596,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9">
         <v>25</v>
@@ -4634,7 +4631,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10">
         <v>15</v>
@@ -4669,7 +4666,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11">
         <v>32</v>
@@ -4704,7 +4701,7 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12">
         <v>18</v>
@@ -4739,7 +4736,7 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D13">
         <v>28</v>
@@ -4774,7 +4771,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14">
         <v>13</v>
@@ -4809,7 +4806,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D15">
         <v>16</v>
@@ -4844,7 +4841,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16">
         <v>11</v>
@@ -4879,7 +4876,7 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17">
         <v>14</v>
@@ -4914,7 +4911,7 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18">
         <v>11</v>
@@ -4949,7 +4946,7 @@
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19">
         <v>17</v>
@@ -4984,7 +4981,7 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D20">
         <v>8</v>
@@ -5019,7 +5016,7 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D21">
         <v>13</v>
@@ -5054,7 +5051,7 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22">
         <v>20</v>
@@ -5089,7 +5086,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D23">
         <v>14</v>
@@ -5124,7 +5121,7 @@
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D24">
         <v>19</v>
@@ -5159,7 +5156,7 @@
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25">
         <v>18</v>
@@ -5194,7 +5191,7 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26">
         <v>21</v>
@@ -5229,7 +5226,7 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27">
         <v>19</v>
@@ -5264,7 +5261,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D28">
         <v>18</v>
@@ -5299,7 +5296,7 @@
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D29">
         <v>25</v>
@@ -5334,7 +5331,7 @@
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30">
         <v>25</v>
@@ -5369,7 +5366,7 @@
         <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D31">
         <v>14</v>
@@ -5404,7 +5401,7 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D32">
         <v>28</v>
@@ -5439,7 +5436,7 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D33">
         <v>15</v>
@@ -5474,7 +5471,7 @@
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34">
         <v>15</v>
@@ -5509,7 +5506,7 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D35">
         <v>15</v>
@@ -5544,7 +5541,7 @@
         <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D36">
         <v>20</v>
@@ -5579,7 +5576,7 @@
         <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D37">
         <v>14</v>
@@ -5614,7 +5611,7 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D38">
         <v>27</v>
@@ -5649,7 +5646,7 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D39">
         <v>23</v>
@@ -5684,7 +5681,7 @@
         <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D40">
         <v>25</v>
@@ -5719,7 +5716,7 @@
         <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D41">
         <v>19</v>
@@ -5754,7 +5751,7 @@
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D42">
         <v>28</v>
@@ -5789,7 +5786,7 @@
         <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D43">
         <v>21</v>
@@ -5824,7 +5821,7 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D44">
         <v>23</v>
@@ -5859,7 +5856,7 @@
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D45">
         <v>15</v>
@@ -5894,7 +5891,7 @@
         <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D46">
         <v>29</v>
@@ -5929,7 +5926,7 @@
         <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D47">
         <v>12</v>
@@ -5964,7 +5961,7 @@
         <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D48">
         <v>43</v>
@@ -5999,7 +5996,7 @@
         <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D49">
         <v>20</v>
@@ -6175,7 +6172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25945CFA-468F-CA47-B44C-691BD86151A8}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -6193,13 +6190,13 @@
         <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -6208,13 +6205,13 @@
         <v>49</v>
       </c>
       <c r="G1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K1" t="s">
         <v>48</v>
@@ -6228,22 +6225,22 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -6254,22 +6251,22 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -6280,7 +6277,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
@@ -6289,13 +6286,13 @@
         <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -6306,7 +6303,7 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -6315,13 +6312,13 @@
         <v>28</v>
       </c>
       <c r="G5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" t="s">
         <v>51</v>
       </c>
-      <c r="H5" t="s">
-        <v>52</v>
-      </c>
       <c r="I5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -6332,22 +6329,22 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
       </c>
       <c r="G6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" t="s">
         <v>51</v>
       </c>
-      <c r="H6" t="s">
-        <v>52</v>
-      </c>
       <c r="I6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>16</v>
@@ -6361,7 +6358,7 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
         <v>20</v>
@@ -6370,13 +6367,13 @@
         <v>21</v>
       </c>
       <c r="G7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" t="s">
         <v>51</v>
       </c>
-      <c r="H7" t="s">
-        <v>52</v>
-      </c>
       <c r="I7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>19</v>
@@ -6390,7 +6387,7 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" t="s">
         <v>47</v>
@@ -6399,13 +6396,13 @@
         <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -6413,10 +6410,10 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
         <v>27</v>
@@ -6425,13 +6422,13 @@
         <v>29</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -6439,28 +6436,28 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F10" t="s">
         <v>29</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -6468,10 +6465,10 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
@@ -6480,13 +6477,13 @@
         <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="H11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>34</v>
@@ -6500,22 +6497,22 @@
         <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E12" t="s">
         <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>